<commit_message>
Added data and documents to Tef validation set
</commit_message>
<xml_diff>
--- a/Prototypes/Tef/Observed.xlsx
+++ b/Prototypes/Tef/Observed.xlsx
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="L64" authorId="0">
+    <comment ref="N64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L67" authorId="0">
+    <comment ref="N67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
   <si>
     <t>SimulationName</t>
   </si>
@@ -314,13 +314,79 @@
   </si>
   <si>
     <t>BiomassN</t>
+  </si>
+  <si>
+    <t>Habro2012Control</t>
+  </si>
+  <si>
+    <t>Habro2012N46S1</t>
+  </si>
+  <si>
+    <t>Habro2012N69S1</t>
+  </si>
+  <si>
+    <t>Habro2012N92S1</t>
+  </si>
+  <si>
+    <t>Habro2012N46S2</t>
+  </si>
+  <si>
+    <t>Habro2012N69S2</t>
+  </si>
+  <si>
+    <t>Habro2012N92S2</t>
+  </si>
+  <si>
+    <t>Habro2012N46S3</t>
+  </si>
+  <si>
+    <t>Habro2012N69S3</t>
+  </si>
+  <si>
+    <t>Habro2012N92S3</t>
+  </si>
+  <si>
+    <t>Habro2012N46S4</t>
+  </si>
+  <si>
+    <t>Habro2012N69S4</t>
+  </si>
+  <si>
+    <t>Habro2012N92S4</t>
+  </si>
+  <si>
+    <t>Habro2012N46S5</t>
+  </si>
+  <si>
+    <t>Habro2012N69S5</t>
+  </si>
+  <si>
+    <t>Habro2012N92S5</t>
+  </si>
+  <si>
+    <t>PanicleSeedWt</t>
+  </si>
+  <si>
+    <t>NoEffectiveTillers</t>
+  </si>
+  <si>
+    <t>PlantHeight</t>
+  </si>
+  <si>
+    <t>LodgingIndex</t>
+  </si>
+  <si>
+    <t>StrawWt</t>
+  </si>
+  <si>
+    <t>StrawN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +406,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -362,12 +435,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,20 +736,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -692,31 +772,49 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -731,22 +829,30 @@
         <v>760</v>
       </c>
       <c r="F2">
+        <f>D2-E2</f>
+        <v>1437</v>
+      </c>
+      <c r="G2">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>20.2</v>
       </c>
-      <c r="K2">
+      <c r="I2">
+        <f>H2-G2</f>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="M2">
         <v>68.7</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>76.7</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -760,22 +866,30 @@
         <v>1158</v>
       </c>
       <c r="F3">
+        <f t="shared" ref="F3:F11" si="0">D3-E3</f>
+        <v>2012</v>
+      </c>
+      <c r="G3">
         <v>31.7</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>41.4</v>
       </c>
-      <c r="K3">
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="1">H3-G3</f>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M3">
         <v>72</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>81.3</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>142.30000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -789,22 +903,30 @@
         <v>1963</v>
       </c>
       <c r="F4">
+        <f t="shared" si="0"/>
+        <v>3045</v>
+      </c>
+      <c r="G4">
         <v>48.3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>62</v>
       </c>
-      <c r="K4">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>13.700000000000003</v>
+      </c>
+      <c r="M4">
         <v>76</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>85</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>146.30000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -818,22 +940,30 @@
         <v>2539</v>
       </c>
       <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4355</v>
+      </c>
+      <c r="G5">
         <v>62.5</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>81.2</v>
       </c>
-      <c r="K5">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>18.700000000000003</v>
+      </c>
+      <c r="M5">
         <v>80.7</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>90</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -847,22 +977,30 @@
         <v>2118</v>
       </c>
       <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3059</v>
+      </c>
+      <c r="G6">
         <v>46.6</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>61.6</v>
       </c>
-      <c r="K6">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="M6">
         <v>74</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>83.3</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -876,26 +1014,34 @@
         <v>2111</v>
       </c>
       <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3608</v>
+      </c>
+      <c r="G7">
         <v>24.7</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>70.5</v>
       </c>
       <c r="I7">
-        <f>E7/10/J7</f>
+        <f t="shared" si="1"/>
+        <v>45.8</v>
+      </c>
+      <c r="K7">
+        <f>E7/10/L7</f>
         <v>844400</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>56.3</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>85.7</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -909,26 +1055,34 @@
         <v>2831</v>
       </c>
       <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5073</v>
+      </c>
+      <c r="G8">
         <v>63.69</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>119.49</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I11" si="0">E8/10/J8</f>
+        <f t="shared" si="1"/>
+        <v>55.8</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K11" si="2">E8/10/L8</f>
         <v>1048518.5185185185</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>2.7E-4</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>58</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>88.3</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -942,26 +1096,34 @@
         <v>3380</v>
       </c>
       <c r="F9">
+        <f t="shared" si="0"/>
+        <v>6012</v>
+      </c>
+      <c r="G9">
         <v>87.19</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>167.19</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
         <v>1090322.5806451612</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>3.1E-4</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>60.7</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -975,26 +1137,34 @@
         <v>3444</v>
       </c>
       <c r="F10">
+        <f t="shared" si="0"/>
+        <v>6208</v>
+      </c>
+      <c r="G10">
         <v>92.29</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>205.89</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>113.59999999999998</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
         <v>984000</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>3.5E-4</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>61.7</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>91.7</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1008,26 +1178,34 @@
         <v>2918</v>
       </c>
       <c r="F11">
+        <f t="shared" si="0"/>
+        <v>5120</v>
+      </c>
+      <c r="G11">
         <v>70.599999999999994</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>131.5</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>60.900000000000006</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
         <v>1042142.8571428573</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>57.3</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>88.7</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:19">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1038,7 +1216,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:19">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1227,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:19">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1060,7 +1238,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:19">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1071,7 +1249,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1258,7 +1436,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1269,7 +1447,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1458,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -1291,7 +1469,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1302,7 +1480,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1313,7 +1491,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1324,7 +1502,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1513,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -1346,7 +1524,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1535,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1368,7 +1546,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
@@ -1379,7 +1557,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -1392,8 +1570,12 @@
       <c r="E44">
         <v>3300</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <f t="shared" ref="F44:F83" si="3">D44-E44</f>
+        <v>10700</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
@@ -1406,8 +1588,12 @@
       <c r="E45">
         <v>3180</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>8020</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
@@ -1420,8 +1606,12 @@
       <c r="E46">
         <v>2520</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>4180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
         <v>56</v>
       </c>
@@ -1434,8 +1624,12 @@
       <c r="E47">
         <v>660</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
         <v>57</v>
       </c>
@@ -1448,8 +1642,12 @@
       <c r="E48">
         <v>2860</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
@@ -1462,8 +1660,12 @@
       <c r="E49">
         <v>2730</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>5470</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="2" t="s">
         <v>59</v>
       </c>
@@ -1476,8 +1678,12 @@
       <c r="E50">
         <v>2320</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>5680</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
@@ -1490,8 +1696,12 @@
       <c r="E51">
         <v>3170</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>7830</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="2" t="s">
         <v>61</v>
       </c>
@@ -1504,8 +1714,12 @@
       <c r="E52">
         <v>2970</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
@@ -1518,8 +1732,12 @@
       <c r="E53">
         <v>2740</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>6260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
@@ -1532,8 +1750,12 @@
       <c r="E54">
         <v>2540</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="F54">
+        <f t="shared" si="3"/>
+        <v>9460</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -1546,8 +1768,12 @@
       <c r="E55">
         <v>3130</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="F55">
+        <f t="shared" si="3"/>
+        <v>8170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
@@ -1560,8 +1786,12 @@
       <c r="E56">
         <v>3110</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="F56">
+        <f t="shared" si="3"/>
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
@@ -1574,8 +1804,12 @@
       <c r="E57">
         <v>2770</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="F57">
+        <f t="shared" si="3"/>
+        <v>7230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="2" t="s">
         <v>67</v>
       </c>
@@ -1588,8 +1822,12 @@
       <c r="E58">
         <v>2550</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="F58">
+        <f t="shared" si="3"/>
+        <v>8950</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="2" t="s">
         <v>68</v>
       </c>
@@ -1602,8 +1840,12 @@
       <c r="E59">
         <v>2940</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="F59">
+        <f t="shared" si="3"/>
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="2" t="s">
         <v>69</v>
       </c>
@@ -1616,8 +1858,12 @@
       <c r="E60">
         <v>640</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="F60">
+        <f t="shared" si="3"/>
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
@@ -1630,8 +1876,12 @@
       <c r="E61">
         <v>730</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="F61">
+        <f t="shared" si="3"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
         <v>71</v>
       </c>
@@ -1644,8 +1894,12 @@
       <c r="E62">
         <v>970</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="F62">
+        <f t="shared" si="3"/>
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -1658,8 +1912,12 @@
       <c r="E63">
         <v>1170</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="F63">
+        <f t="shared" si="3"/>
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -1672,14 +1930,18 @@
       <c r="E64">
         <v>1950</v>
       </c>
-      <c r="L64">
+      <c r="F64">
+        <f t="shared" si="3"/>
+        <v>5670</v>
+      </c>
+      <c r="N64">
         <v>46</v>
       </c>
-      <c r="M64">
+      <c r="O64">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:19">
       <c r="A65" s="2" t="s">
         <v>74</v>
       </c>
@@ -1692,8 +1954,12 @@
       <c r="E65">
         <v>370</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="F65">
+        <f t="shared" si="3"/>
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="2" t="s">
         <v>75</v>
       </c>
@@ -1706,8 +1972,12 @@
       <c r="E66">
         <v>610</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="F66">
+        <f t="shared" si="3"/>
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" s="2" t="s">
         <v>76</v>
       </c>
@@ -1720,11 +1990,728 @@
       <c r="E67">
         <v>1400</v>
       </c>
-      <c r="L67">
+      <c r="F67">
+        <f t="shared" si="3"/>
+        <v>4400</v>
+      </c>
+      <c r="N67">
         <v>44</v>
       </c>
-      <c r="M67">
+      <c r="O67">
         <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
+      <c r="A68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>4857</v>
+      </c>
+      <c r="E68">
+        <v>1605.83</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>3251.17</v>
+      </c>
+      <c r="G68">
+        <v>18.3</v>
+      </c>
+      <c r="H68">
+        <v>31.5</v>
+      </c>
+      <c r="I68">
+        <f t="shared" ref="I68:I83" si="4">H68-G68</f>
+        <v>13.2</v>
+      </c>
+      <c r="K68">
+        <f>E12/10/L68</f>
+        <v>1008316.0083160083</v>
+      </c>
+      <c r="L68">
+        <v>2.8860000000000002E-4</v>
+      </c>
+      <c r="M68">
+        <v>48</v>
+      </c>
+      <c r="O68">
+        <v>84.8</v>
+      </c>
+      <c r="P68">
+        <v>5.47</v>
+      </c>
+      <c r="Q68">
+        <v>7.73</v>
+      </c>
+      <c r="R68">
+        <v>95.75</v>
+      </c>
+      <c r="S68">
+        <v>28.85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
+      <c r="A69" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3">
+        <v>6011</v>
+      </c>
+      <c r="E69" s="3">
+        <v>1795</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>4216</v>
+      </c>
+      <c r="G69" s="3">
+        <v>24.53</v>
+      </c>
+      <c r="H69" s="3">
+        <v>46.24</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="4"/>
+        <v>21.71</v>
+      </c>
+      <c r="M69" s="3">
+        <v>49.33</v>
+      </c>
+      <c r="P69" s="3">
+        <v>4.67</v>
+      </c>
+      <c r="Q69" s="3">
+        <v>11.33</v>
+      </c>
+      <c r="R69" s="3">
+        <v>112.58</v>
+      </c>
+      <c r="S69" s="3">
+        <v>34.43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
+      <c r="A70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3">
+        <v>6520</v>
+      </c>
+      <c r="E70" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>4497</v>
+      </c>
+      <c r="G70" s="3">
+        <v>25.24</v>
+      </c>
+      <c r="H70" s="3">
+        <v>45.94</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="4"/>
+        <v>20.7</v>
+      </c>
+      <c r="M70" s="3">
+        <v>53.33</v>
+      </c>
+      <c r="P70" s="3">
+        <v>5.33</v>
+      </c>
+      <c r="Q70" s="3">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="R70" s="3">
+        <v>113.25</v>
+      </c>
+      <c r="S70" s="3">
+        <v>36.44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
+      <c r="A71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3">
+        <v>6708</v>
+      </c>
+      <c r="E71" s="3">
+        <v>1818</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>4890</v>
+      </c>
+      <c r="G71" s="3">
+        <v>27.2</v>
+      </c>
+      <c r="H71" s="3">
+        <v>57.84</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="4"/>
+        <v>30.640000000000004</v>
+      </c>
+      <c r="M71" s="3">
+        <v>52</v>
+      </c>
+      <c r="P71" s="3">
+        <v>7.33</v>
+      </c>
+      <c r="Q71" s="3">
+        <v>17</v>
+      </c>
+      <c r="R71" s="3">
+        <v>112.22</v>
+      </c>
+      <c r="S71" s="3">
+        <v>47.88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
+      <c r="A72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3">
+        <v>7061</v>
+      </c>
+      <c r="E72" s="3">
+        <v>2087</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>4974</v>
+      </c>
+      <c r="G72" s="3">
+        <v>27.61</v>
+      </c>
+      <c r="H72" s="3">
+        <v>50.72</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="4"/>
+        <v>23.11</v>
+      </c>
+      <c r="M72" s="3">
+        <v>52.67</v>
+      </c>
+      <c r="P72" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>15</v>
+      </c>
+      <c r="R72" s="3">
+        <v>113.41</v>
+      </c>
+      <c r="S72" s="3">
+        <v>41.15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
+      <c r="A73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3">
+        <v>6775</v>
+      </c>
+      <c r="E73" s="3">
+        <v>2063</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>4712</v>
+      </c>
+      <c r="G73" s="3">
+        <v>29.28</v>
+      </c>
+      <c r="H73" s="3">
+        <v>59.99</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="4"/>
+        <v>30.71</v>
+      </c>
+      <c r="M73" s="3">
+        <v>54</v>
+      </c>
+      <c r="P73" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q73" s="3">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="R73" s="3">
+        <v>116.7</v>
+      </c>
+      <c r="S73" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
+      <c r="A74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3">
+        <v>6825</v>
+      </c>
+      <c r="E74" s="3">
+        <v>2083</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>4742</v>
+      </c>
+      <c r="G74" s="3">
+        <v>32.270000000000003</v>
+      </c>
+      <c r="H74" s="3">
+        <v>65.22</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="4"/>
+        <v>32.949999999999996</v>
+      </c>
+      <c r="M74" s="3">
+        <v>54</v>
+      </c>
+      <c r="P74" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="Q74" s="3">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="R74" s="3">
+        <v>117.53</v>
+      </c>
+      <c r="S74" s="3">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
+      <c r="A75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3">
+        <v>7433</v>
+      </c>
+      <c r="E75" s="3">
+        <v>2197</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>5236</v>
+      </c>
+      <c r="G75" s="3">
+        <v>27.12</v>
+      </c>
+      <c r="H75" s="3">
+        <v>49.24</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="4"/>
+        <v>22.12</v>
+      </c>
+      <c r="M75" s="3">
+        <v>51.67</v>
+      </c>
+      <c r="P75" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q75" s="3">
+        <v>13</v>
+      </c>
+      <c r="R75" s="3">
+        <v>116.8</v>
+      </c>
+      <c r="S75" s="3">
+        <v>45.96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
+      <c r="A76" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3">
+        <v>9004</v>
+      </c>
+      <c r="E76" s="3">
+        <v>2504</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>6500</v>
+      </c>
+      <c r="G76" s="3">
+        <v>33.979999999999997</v>
+      </c>
+      <c r="H76" s="3">
+        <v>65.78</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="4"/>
+        <v>31.800000000000004</v>
+      </c>
+      <c r="M76" s="3">
+        <v>51.33</v>
+      </c>
+      <c r="P76" s="3">
+        <v>8.67</v>
+      </c>
+      <c r="Q76" s="3">
+        <v>20.67</v>
+      </c>
+      <c r="R76" s="3">
+        <v>120.95</v>
+      </c>
+      <c r="S76" s="3">
+        <v>46.91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
+      <c r="A77" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3">
+        <v>6307</v>
+      </c>
+      <c r="E77" s="3">
+        <v>2065</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>4242</v>
+      </c>
+      <c r="G77" s="3">
+        <v>31.38</v>
+      </c>
+      <c r="H77" s="3">
+        <v>60.02</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="4"/>
+        <v>28.640000000000004</v>
+      </c>
+      <c r="M77" s="3">
+        <v>51</v>
+      </c>
+      <c r="P77" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q77" s="3">
+        <v>16</v>
+      </c>
+      <c r="R77" s="3">
+        <v>119.07</v>
+      </c>
+      <c r="S77" s="3">
+        <v>46.91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
+      <c r="A78" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3">
+        <v>6181</v>
+      </c>
+      <c r="E78" s="3">
+        <v>1657</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>4524</v>
+      </c>
+      <c r="G78" s="3">
+        <v>22.63</v>
+      </c>
+      <c r="H78" s="3">
+        <v>41.72</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="4"/>
+        <v>19.09</v>
+      </c>
+      <c r="M78" s="3">
+        <v>52.33</v>
+      </c>
+      <c r="P78" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q78" s="3">
+        <v>14.33</v>
+      </c>
+      <c r="R78" s="3">
+        <v>116.23</v>
+      </c>
+      <c r="S78" s="3">
+        <v>37.659999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
+      <c r="A79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3">
+        <v>8296</v>
+      </c>
+      <c r="E79" s="3">
+        <v>2266</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>6030</v>
+      </c>
+      <c r="G79" s="3">
+        <v>32.58</v>
+      </c>
+      <c r="H79" s="3">
+        <v>64.73</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="4"/>
+        <v>32.150000000000006</v>
+      </c>
+      <c r="M79" s="3">
+        <v>51.67</v>
+      </c>
+      <c r="P79" s="3">
+        <v>8.67</v>
+      </c>
+      <c r="Q79" s="3">
+        <v>13</v>
+      </c>
+      <c r="R79" s="3">
+        <v>117.1</v>
+      </c>
+      <c r="S79" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
+      <c r="A80" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3">
+        <v>5914</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1850</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>4064</v>
+      </c>
+      <c r="G80" s="3">
+        <v>27</v>
+      </c>
+      <c r="H80" s="3">
+        <v>51.83</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="4"/>
+        <v>24.83</v>
+      </c>
+      <c r="M80" s="3">
+        <v>54</v>
+      </c>
+      <c r="P80" s="3">
+        <v>5.67</v>
+      </c>
+      <c r="Q80" s="3">
+        <v>16</v>
+      </c>
+      <c r="R80" s="3">
+        <v>119</v>
+      </c>
+      <c r="S80" s="3">
+        <v>42.12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
+      <c r="A81" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3">
+        <v>6093</v>
+      </c>
+      <c r="E81" s="3">
+        <v>1878</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>4215</v>
+      </c>
+      <c r="G81" s="3">
+        <v>23.69</v>
+      </c>
+      <c r="H81" s="3">
+        <v>43.4</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="4"/>
+        <v>19.709999999999997</v>
+      </c>
+      <c r="M81" s="3">
+        <v>53.67</v>
+      </c>
+      <c r="P81" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q81" s="3">
+        <v>9</v>
+      </c>
+      <c r="R81" s="3">
+        <v>114.92</v>
+      </c>
+      <c r="S81" s="3">
+        <v>38.44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
+      <c r="A82" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3">
+        <v>7830</v>
+      </c>
+      <c r="E82" s="3">
+        <v>2402</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>5428</v>
+      </c>
+      <c r="G82" s="3">
+        <v>33.26</v>
+      </c>
+      <c r="H82" s="3">
+        <v>54.95</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="4"/>
+        <v>21.690000000000005</v>
+      </c>
+      <c r="M82" s="3">
+        <v>50.67</v>
+      </c>
+      <c r="P82" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q82" s="3">
+        <v>12.67</v>
+      </c>
+      <c r="R82" s="3">
+        <v>117.8</v>
+      </c>
+      <c r="S82" s="3">
+        <v>43.09</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
+      <c r="A83" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3">
+        <v>7630</v>
+      </c>
+      <c r="E83" s="3">
+        <v>2212</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>5418</v>
+      </c>
+      <c r="G83" s="3">
+        <v>29.46</v>
+      </c>
+      <c r="H83" s="3">
+        <v>52.77</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="4"/>
+        <v>23.310000000000002</v>
+      </c>
+      <c r="M83" s="3">
+        <v>54.67</v>
+      </c>
+      <c r="P83" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q83" s="3">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="R83" s="3">
+        <v>118.27</v>
+      </c>
+      <c r="S83" s="3">
+        <v>41.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on Tef Model
</commit_message>
<xml_diff>
--- a/Prototypes/Tef/Observed.xlsx
+++ b/Prototypes/Tef/Observed.xlsx
@@ -235,54 +235,6 @@
     <t>CWP2010PopHighTreatment16</t>
   </si>
   <si>
-    <t>CWP2011PopHighTreatment1</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment2</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment3</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment4</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment5</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment6</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment7</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment8</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment9</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment10</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment11</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment12</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment13</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment14</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment15</t>
-  </si>
-  <si>
-    <t>CWP2011PopHighTreatment16</t>
-  </si>
-  <si>
     <t>Mekelle2008Irrigation0</t>
   </si>
   <si>
@@ -380,6 +332,54 @@
   </si>
   <si>
     <t>StrawN</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment1</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment2</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment3</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment4</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment5</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment6</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment7</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment8</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment9</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment10</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment11</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment12</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment13</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment14</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment15</t>
+  </si>
+  <si>
+    <t>CWP2011Treatment16</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
   <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <pane xSplit="5400" ySplit="576" topLeftCell="B37" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <selection pane="bottomRight" activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -772,16 +772,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -793,7 +793,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s">
         <v>8</v>
@@ -802,16 +802,16 @@
         <v>9</v>
       </c>
       <c r="P1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="R1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="S1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -823,14 +823,13 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
-        <v>2197</v>
+        <v>219.7</v>
       </c>
       <c r="E2">
-        <v>760</v>
+        <v>76</v>
       </c>
       <c r="F2">
-        <f>D2-E2</f>
-        <v>1437</v>
+        <v>143.69999999999999</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -860,14 +859,13 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>3170</v>
+        <v>317</v>
       </c>
       <c r="E3">
-        <v>1158</v>
+        <v>115.8</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="0">D3-E3</f>
-        <v>2012</v>
+        <v>201.2</v>
       </c>
       <c r="G3">
         <v>31.7</v>
@@ -876,7 +874,7 @@
         <v>41.4</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="1">H3-G3</f>
+        <f t="shared" ref="I3:I11" si="0">H3-G3</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="M3">
@@ -897,14 +895,13 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>5008</v>
+        <v>500.8</v>
       </c>
       <c r="E4">
-        <v>1963</v>
+        <v>196.3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>3045</v>
+        <v>304.5</v>
       </c>
       <c r="G4">
         <v>48.3</v>
@@ -913,7 +910,7 @@
         <v>62</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13.700000000000003</v>
       </c>
       <c r="M4">
@@ -934,14 +931,13 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>6894</v>
+        <v>689.4</v>
       </c>
       <c r="E5">
-        <v>2539</v>
+        <v>253.9</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>4355</v>
+        <v>435.5</v>
       </c>
       <c r="G5">
         <v>62.5</v>
@@ -950,7 +946,7 @@
         <v>81.2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18.700000000000003</v>
       </c>
       <c r="M5">
@@ -971,14 +967,13 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>5177</v>
+        <v>517.70000000000005</v>
       </c>
       <c r="E6">
-        <v>2118</v>
+        <v>211.8</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>3059</v>
+        <v>305.89999999999998</v>
       </c>
       <c r="G6">
         <v>46.6</v>
@@ -987,7 +982,7 @@
         <v>61.6</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M6">
@@ -1008,14 +1003,13 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>5719</v>
+        <v>571.9</v>
       </c>
       <c r="E7">
-        <v>2111</v>
+        <v>211.1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>3608</v>
+        <v>360.8</v>
       </c>
       <c r="G7">
         <v>24.7</v>
@@ -1024,12 +1018,12 @@
         <v>70.5</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45.8</v>
       </c>
       <c r="K7">
         <f>E7/10/L7</f>
-        <v>844400</v>
+        <v>84440</v>
       </c>
       <c r="L7">
         <v>2.5000000000000001E-4</v>
@@ -1049,14 +1043,13 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>7904</v>
+        <v>790.4</v>
       </c>
       <c r="E8">
-        <v>2831</v>
+        <v>283.10000000000002</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>5073</v>
+        <v>507.3</v>
       </c>
       <c r="G8">
         <v>63.69</v>
@@ -1065,12 +1058,12 @@
         <v>119.49</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55.8</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K11" si="2">E8/10/L8</f>
-        <v>1048518.5185185185</v>
+        <f>E8/10/L8</f>
+        <v>104851.85185185185</v>
       </c>
       <c r="L8">
         <v>2.7E-4</v>
@@ -1090,14 +1083,13 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>9392</v>
+        <v>939.2</v>
       </c>
       <c r="E9">
-        <v>3380</v>
+        <v>338</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>6012</v>
+        <v>601.20000000000005</v>
       </c>
       <c r="G9">
         <v>87.19</v>
@@ -1106,12 +1098,12 @@
         <v>167.19</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
-        <v>1090322.5806451612</v>
+        <f>E9/10/L9</f>
+        <v>109032.25806451612</v>
       </c>
       <c r="L9">
         <v>3.1E-4</v>
@@ -1131,14 +1123,13 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>9652</v>
+        <v>965.2</v>
       </c>
       <c r="E10">
-        <v>3444</v>
+        <v>344.4</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>6208</v>
+        <v>620.79999999999995</v>
       </c>
       <c r="G10">
         <v>92.29</v>
@@ -1147,12 +1138,12 @@
         <v>205.89</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>113.59999999999998</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>984000</v>
+        <f>E10/10/L10</f>
+        <v>98400</v>
       </c>
       <c r="L10">
         <v>3.5E-4</v>
@@ -1172,14 +1163,13 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>8038</v>
+        <v>803.8</v>
       </c>
       <c r="E11">
-        <v>2918</v>
+        <v>291.8</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>5120</v>
+        <v>512</v>
       </c>
       <c r="G11">
         <v>70.599999999999994</v>
@@ -1188,12 +1178,12 @@
         <v>131.5</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60.900000000000006</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>1042142.8571428573</v>
+        <f>E11/10/L11</f>
+        <v>104214.28571428572</v>
       </c>
       <c r="L11">
         <v>2.7999999999999998E-4</v>
@@ -1213,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>2910</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1224,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <v>2270</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1235,7 +1225,7 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>960</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1246,7 +1236,7 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>450</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1257,7 +1247,7 @@
         <v>10</v>
       </c>
       <c r="E16">
-        <v>1620</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1268,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="E17">
-        <v>1780</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1279,7 +1269,7 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <v>1100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1290,7 +1280,7 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>2100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1301,7 +1291,7 @@
         <v>10</v>
       </c>
       <c r="E20">
-        <v>2520</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1312,7 +1302,7 @@
         <v>10</v>
       </c>
       <c r="E21">
-        <v>1990</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1323,7 +1313,7 @@
         <v>10</v>
       </c>
       <c r="E22">
-        <v>1490</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1334,7 +1324,7 @@
         <v>10</v>
       </c>
       <c r="E23">
-        <v>2360</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1345,7 +1335,7 @@
         <v>10</v>
       </c>
       <c r="E24">
-        <v>2810</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1356,7 +1346,7 @@
         <v>10</v>
       </c>
       <c r="E25">
-        <v>2490</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1367,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="E26">
-        <v>1930</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1378,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="E27">
-        <v>2850</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1389,7 +1379,7 @@
         <v>10</v>
       </c>
       <c r="E28">
-        <v>3120</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1400,7 +1390,7 @@
         <v>10</v>
       </c>
       <c r="E29">
-        <v>2450</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1411,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="E30">
-        <v>1510</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1422,7 +1412,7 @@
         <v>10</v>
       </c>
       <c r="E31">
-        <v>690</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1433,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="E32">
-        <v>2020</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1444,7 +1434,7 @@
         <v>10</v>
       </c>
       <c r="E33">
-        <v>2200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1455,7 +1445,7 @@
         <v>10</v>
       </c>
       <c r="E34">
-        <v>1520</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1466,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="E35">
-        <v>2430</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1477,7 +1467,7 @@
         <v>10</v>
       </c>
       <c r="E36">
-        <v>2980</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1488,7 +1478,7 @@
         <v>10</v>
       </c>
       <c r="E37">
-        <v>2420</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1499,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="E38">
-        <v>1950</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1510,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="E39">
-        <v>2750</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1521,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="E40">
-        <v>3090</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1532,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E41">
-        <v>2800</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1543,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="E42">
-        <v>2350</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1554,385 +1544,364 @@
         <v>10</v>
       </c>
       <c r="E43">
-        <v>3000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
       </c>
       <c r="D44">
-        <v>14000</v>
+        <v>1400</v>
       </c>
       <c r="E44">
-        <v>3300</v>
+        <v>330</v>
       </c>
       <c r="F44">
-        <f t="shared" ref="F44:F83" si="3">D44-E44</f>
-        <v>10700</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
       </c>
       <c r="D45">
-        <v>11200</v>
+        <v>1120</v>
       </c>
       <c r="E45">
-        <v>3180</v>
+        <v>318</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
-        <v>8020</v>
+        <v>802</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
       <c r="D46">
-        <v>6700</v>
+        <v>670</v>
       </c>
       <c r="E46">
-        <v>2520</v>
+        <v>252</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
-        <v>4180</v>
+        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
       </c>
       <c r="D47">
-        <v>4500</v>
+        <v>450</v>
       </c>
       <c r="E47">
-        <v>660</v>
+        <v>66</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
-        <v>3840</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="D48">
-        <v>6200</v>
+        <v>620</v>
       </c>
       <c r="E48">
-        <v>2860</v>
+        <v>286</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
-        <v>3340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
       </c>
       <c r="D49">
-        <v>8200</v>
+        <v>820</v>
       </c>
       <c r="E49">
-        <v>2730</v>
+        <v>273</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
-        <v>5470</v>
+        <v>547</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="2" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
       </c>
       <c r="D50">
-        <v>8000</v>
+        <v>800</v>
       </c>
       <c r="E50">
-        <v>2320</v>
+        <v>232</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
-        <v>5680</v>
+        <v>568</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
       </c>
       <c r="D51">
-        <v>11000</v>
+        <v>1100</v>
       </c>
       <c r="E51">
-        <v>3170</v>
+        <v>317</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
-        <v>7830</v>
+        <v>783</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
       <c r="D52">
-        <v>6700</v>
+        <v>670</v>
       </c>
       <c r="E52">
-        <v>2970</v>
+        <v>297</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
-        <v>3730</v>
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="2" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
       <c r="D53">
-        <v>9000</v>
+        <v>900</v>
       </c>
       <c r="E53">
-        <v>2740</v>
+        <v>274</v>
       </c>
       <c r="F53">
-        <f t="shared" si="3"/>
-        <v>6260</v>
+        <v>626</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="2" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
       <c r="D54">
-        <v>12000</v>
+        <v>1200</v>
       </c>
       <c r="E54">
-        <v>2540</v>
+        <v>254</v>
       </c>
       <c r="F54">
-        <f t="shared" si="3"/>
-        <v>9460</v>
+        <v>946</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="2" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
       <c r="D55">
-        <v>11300</v>
+        <v>1130</v>
       </c>
       <c r="E55">
-        <v>3130</v>
+        <v>313</v>
       </c>
       <c r="F55">
-        <f t="shared" si="3"/>
-        <v>8170</v>
+        <v>817</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
       <c r="D56">
-        <v>8800</v>
+        <v>880</v>
       </c>
       <c r="E56">
-        <v>3110</v>
+        <v>311</v>
       </c>
       <c r="F56">
-        <f t="shared" si="3"/>
-        <v>5690</v>
+        <v>569</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="D57">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E57">
-        <v>2770</v>
+        <v>277</v>
       </c>
       <c r="F57">
-        <f t="shared" si="3"/>
-        <v>7230</v>
+        <v>723</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
       </c>
       <c r="D58">
-        <v>11500</v>
+        <v>1150</v>
       </c>
       <c r="E58">
-        <v>2550</v>
+        <v>255</v>
       </c>
       <c r="F58">
-        <f t="shared" si="3"/>
-        <v>8950</v>
+        <v>895</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
       </c>
       <c r="D59">
-        <v>11700</v>
+        <v>1170</v>
       </c>
       <c r="E59">
-        <v>2940</v>
+        <v>294</v>
       </c>
       <c r="F59">
-        <f t="shared" si="3"/>
-        <v>8760</v>
+        <v>876</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
       </c>
       <c r="D60">
-        <v>3930</v>
+        <v>393</v>
       </c>
       <c r="E60">
-        <v>640</v>
+        <v>64</v>
       </c>
       <c r="F60">
-        <f t="shared" si="3"/>
-        <v>3290</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
       <c r="D61">
-        <v>4630</v>
+        <v>463</v>
       </c>
       <c r="E61">
-        <v>730</v>
+        <v>73</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
-        <v>3900</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
       </c>
       <c r="D62">
-        <v>5400</v>
+        <v>540</v>
       </c>
       <c r="E62">
-        <v>970</v>
+        <v>97</v>
       </c>
       <c r="F62">
-        <f t="shared" si="3"/>
-        <v>4430</v>
+        <v>443</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
       </c>
       <c r="D63">
-        <v>6220</v>
+        <v>622</v>
       </c>
       <c r="E63">
-        <v>1170</v>
+        <v>117</v>
       </c>
       <c r="F63">
-        <f t="shared" si="3"/>
-        <v>5050</v>
+        <v>505</v>
       </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
       <c r="D64">
-        <v>7620</v>
+        <v>762</v>
       </c>
       <c r="E64">
-        <v>1950</v>
+        <v>195</v>
       </c>
       <c r="F64">
-        <f t="shared" si="3"/>
-        <v>5670</v>
+        <v>567</v>
       </c>
       <c r="N64">
         <v>46</v>
@@ -1943,56 +1912,53 @@
     </row>
     <row r="65" spans="1:19">
       <c r="A65" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="D65">
-        <v>3480</v>
+        <v>348</v>
       </c>
       <c r="E65">
-        <v>370</v>
+        <v>37</v>
       </c>
       <c r="F65">
-        <f t="shared" si="3"/>
-        <v>3110</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:19">
       <c r="A66" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
       </c>
       <c r="D66">
-        <v>4530</v>
+        <v>453</v>
       </c>
       <c r="E66">
-        <v>610</v>
+        <v>61</v>
       </c>
       <c r="F66">
-        <f t="shared" si="3"/>
-        <v>3920</v>
+        <v>392</v>
       </c>
     </row>
     <row r="67" spans="1:19">
       <c r="A67" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
       </c>
       <c r="D67">
-        <v>5800</v>
+        <v>580</v>
       </c>
       <c r="E67">
-        <v>1400</v>
+        <v>140</v>
       </c>
       <c r="F67">
-        <f t="shared" si="3"/>
-        <v>4400</v>
+        <v>440</v>
       </c>
       <c r="N67">
         <v>44</v>
@@ -2003,20 +1969,19 @@
     </row>
     <row r="68" spans="1:19">
       <c r="A68" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="D68">
-        <v>4857</v>
+        <v>485.7</v>
       </c>
       <c r="E68">
-        <v>1605.83</v>
+        <v>160.583</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
-        <v>3251.17</v>
+        <v>325.11700000000002</v>
       </c>
       <c r="G68">
         <v>18.3</v>
@@ -2025,12 +1990,12 @@
         <v>31.5</v>
       </c>
       <c r="I68">
-        <f t="shared" ref="I68:I83" si="4">H68-G68</f>
+        <f t="shared" ref="I68:I83" si="1">H68-G68</f>
         <v>13.2</v>
       </c>
       <c r="K68">
         <f>E12/10/L68</f>
-        <v>1008316.0083160083</v>
+        <v>100831.60083160082</v>
       </c>
       <c r="L68">
         <v>2.8860000000000002E-4</v>
@@ -2056,21 +2021,20 @@
     </row>
     <row r="69" spans="1:19">
       <c r="A69" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3">
-        <v>6011</v>
+        <v>601.1</v>
       </c>
       <c r="E69" s="3">
-        <v>1795</v>
+        <v>179.5</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
-        <v>4216</v>
+        <v>421.6</v>
       </c>
       <c r="G69" s="3">
         <v>24.53</v>
@@ -2079,7 +2043,7 @@
         <v>46.24</v>
       </c>
       <c r="I69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>21.71</v>
       </c>
       <c r="M69" s="3">
@@ -2100,21 +2064,20 @@
     </row>
     <row r="70" spans="1:19">
       <c r="A70" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3">
-        <v>6520</v>
+        <v>652</v>
       </c>
       <c r="E70" s="3">
-        <v>2023</v>
+        <v>202.3</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
-        <v>4497</v>
+        <v>449.7</v>
       </c>
       <c r="G70" s="3">
         <v>25.24</v>
@@ -2123,7 +2086,7 @@
         <v>45.94</v>
       </c>
       <c r="I70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>20.7</v>
       </c>
       <c r="M70" s="3">
@@ -2144,21 +2107,20 @@
     </row>
     <row r="71" spans="1:19">
       <c r="A71" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3">
-        <v>6708</v>
+        <v>670.8</v>
       </c>
       <c r="E71" s="3">
-        <v>1818</v>
+        <v>181.8</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
-        <v>4890</v>
+        <v>489</v>
       </c>
       <c r="G71" s="3">
         <v>27.2</v>
@@ -2167,7 +2129,7 @@
         <v>57.84</v>
       </c>
       <c r="I71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>30.640000000000004</v>
       </c>
       <c r="M71" s="3">
@@ -2188,21 +2150,20 @@
     </row>
     <row r="72" spans="1:19">
       <c r="A72" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3">
-        <v>7061</v>
+        <v>706.1</v>
       </c>
       <c r="E72" s="3">
-        <v>2087</v>
+        <v>208.7</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
-        <v>4974</v>
+        <v>497.4</v>
       </c>
       <c r="G72" s="3">
         <v>27.61</v>
@@ -2211,7 +2172,7 @@
         <v>50.72</v>
       </c>
       <c r="I72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>23.11</v>
       </c>
       <c r="M72" s="3">
@@ -2232,21 +2193,20 @@
     </row>
     <row r="73" spans="1:19">
       <c r="A73" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3">
-        <v>6775</v>
+        <v>677.5</v>
       </c>
       <c r="E73" s="3">
-        <v>2063</v>
+        <v>206.3</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
-        <v>4712</v>
+        <v>471.2</v>
       </c>
       <c r="G73" s="3">
         <v>29.28</v>
@@ -2255,7 +2215,7 @@
         <v>59.99</v>
       </c>
       <c r="I73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>30.71</v>
       </c>
       <c r="M73" s="3">
@@ -2276,21 +2236,20 @@
     </row>
     <row r="74" spans="1:19">
       <c r="A74" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3">
-        <v>6825</v>
+        <v>682.5</v>
       </c>
       <c r="E74" s="3">
-        <v>2083</v>
+        <v>208.3</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
-        <v>4742</v>
+        <v>474.2</v>
       </c>
       <c r="G74" s="3">
         <v>32.270000000000003</v>
@@ -2299,7 +2258,7 @@
         <v>65.22</v>
       </c>
       <c r="I74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>32.949999999999996</v>
       </c>
       <c r="M74" s="3">
@@ -2320,21 +2279,20 @@
     </row>
     <row r="75" spans="1:19">
       <c r="A75" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3">
-        <v>7433</v>
+        <v>743.3</v>
       </c>
       <c r="E75" s="3">
-        <v>2197</v>
+        <v>219.7</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
-        <v>5236</v>
+        <v>523.6</v>
       </c>
       <c r="G75" s="3">
         <v>27.12</v>
@@ -2343,7 +2301,7 @@
         <v>49.24</v>
       </c>
       <c r="I75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>22.12</v>
       </c>
       <c r="M75" s="3">
@@ -2364,21 +2322,20 @@
     </row>
     <row r="76" spans="1:19">
       <c r="A76" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3">
-        <v>9004</v>
+        <v>900.4</v>
       </c>
       <c r="E76" s="3">
-        <v>2504</v>
+        <v>250.4</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
-        <v>6500</v>
+        <v>650</v>
       </c>
       <c r="G76" s="3">
         <v>33.979999999999997</v>
@@ -2387,7 +2344,7 @@
         <v>65.78</v>
       </c>
       <c r="I76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>31.800000000000004</v>
       </c>
       <c r="M76" s="3">
@@ -2408,21 +2365,20 @@
     </row>
     <row r="77" spans="1:19">
       <c r="A77" s="2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3">
-        <v>6307</v>
+        <v>630.70000000000005</v>
       </c>
       <c r="E77" s="3">
-        <v>2065</v>
+        <v>206.5</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
-        <v>4242</v>
+        <v>424.2</v>
       </c>
       <c r="G77" s="3">
         <v>31.38</v>
@@ -2431,7 +2387,7 @@
         <v>60.02</v>
       </c>
       <c r="I77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>28.640000000000004</v>
       </c>
       <c r="M77" s="3">
@@ -2452,21 +2408,20 @@
     </row>
     <row r="78" spans="1:19">
       <c r="A78" s="2" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3">
-        <v>6181</v>
+        <v>618.1</v>
       </c>
       <c r="E78" s="3">
-        <v>1657</v>
+        <v>165.7</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
-        <v>4524</v>
+        <v>452.4</v>
       </c>
       <c r="G78" s="3">
         <v>22.63</v>
@@ -2475,7 +2430,7 @@
         <v>41.72</v>
       </c>
       <c r="I78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>19.09</v>
       </c>
       <c r="M78" s="3">
@@ -2496,21 +2451,20 @@
     </row>
     <row r="79" spans="1:19">
       <c r="A79" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3">
-        <v>8296</v>
+        <v>829.6</v>
       </c>
       <c r="E79" s="3">
-        <v>2266</v>
+        <v>226.6</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
-        <v>6030</v>
+        <v>603</v>
       </c>
       <c r="G79" s="3">
         <v>32.58</v>
@@ -2519,7 +2473,7 @@
         <v>64.73</v>
       </c>
       <c r="I79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>32.150000000000006</v>
       </c>
       <c r="M79" s="3">
@@ -2540,21 +2494,20 @@
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3">
-        <v>5914</v>
+        <v>591.4</v>
       </c>
       <c r="E80" s="3">
-        <v>1850</v>
+        <v>185</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
-        <v>4064</v>
+        <v>406.4</v>
       </c>
       <c r="G80" s="3">
         <v>27</v>
@@ -2563,7 +2516,7 @@
         <v>51.83</v>
       </c>
       <c r="I80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>24.83</v>
       </c>
       <c r="M80" s="3">
@@ -2584,21 +2537,20 @@
     </row>
     <row r="81" spans="1:19">
       <c r="A81" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3">
-        <v>6093</v>
+        <v>609.29999999999995</v>
       </c>
       <c r="E81" s="3">
-        <v>1878</v>
+        <v>187.8</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
-        <v>4215</v>
+        <v>421.5</v>
       </c>
       <c r="G81" s="3">
         <v>23.69</v>
@@ -2607,7 +2559,7 @@
         <v>43.4</v>
       </c>
       <c r="I81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>19.709999999999997</v>
       </c>
       <c r="M81" s="3">
@@ -2628,21 +2580,20 @@
     </row>
     <row r="82" spans="1:19">
       <c r="A82" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3">
-        <v>7830</v>
+        <v>783</v>
       </c>
       <c r="E82" s="3">
-        <v>2402</v>
+        <v>240.2</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
-        <v>5428</v>
+        <v>542.79999999999995</v>
       </c>
       <c r="G82" s="3">
         <v>33.26</v>
@@ -2651,7 +2602,7 @@
         <v>54.95</v>
       </c>
       <c r="I82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>21.690000000000005</v>
       </c>
       <c r="M82" s="3">
@@ -2672,21 +2623,20 @@
     </row>
     <row r="83" spans="1:19">
       <c r="A83" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3">
-        <v>7630</v>
+        <v>763</v>
       </c>
       <c r="E83" s="3">
-        <v>2212</v>
+        <v>221.2</v>
       </c>
       <c r="F83">
-        <f t="shared" si="3"/>
-        <v>5418</v>
+        <v>541.79999999999995</v>
       </c>
       <c r="G83" s="3">
         <v>29.46</v>
@@ -2695,7 +2645,7 @@
         <v>52.77</v>
       </c>
       <c r="I83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>23.310000000000002</v>
       </c>
       <c r="M83" s="3">

</xml_diff>